<commit_message>
Add refined charts, completed notebook, input files
</commit_message>
<xml_diff>
--- a/output_data/charts/0500000US39041.xlsx
+++ b/output_data/charts/0500000US39041.xlsx
@@ -141,11 +141,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100"/>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -199,40 +211,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>4.581090895547403</c:v>
+                  <c:v>4.562468574833796</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.581103570702121</c:v>
+                  <c:v>4.585883614711811</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.612300651043976</c:v>
+                  <c:v>4.576821415266715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.674182018146825</c:v>
+                  <c:v>4.669026670332691</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.672935947192092</c:v>
+                  <c:v>4.660496898530534</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.833134684147796</c:v>
+                  <c:v>4.814628944231855</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.074002373071879</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.05750889044296</c:v>
+                  <c:v>5.021798324579286</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.306948779540584</c:v>
+                  <c:v>5.250061130848784</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.728086415456785</c:v>
+                  <c:v>5.71089519620262</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.008419441255263</c:v>
+                  <c:v>6.070443538276786</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.294934746091226</c:v>
+                  <c:v>6.294934746091227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,7 +267,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" baseline="0"/>
+              <a:defRPr sz="1600" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -270,7 +284,7 @@
         <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6.9244282207003485"/>
+          <c:max val="7"/>
           <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -282,7 +296,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" baseline="0"/>
+              <a:defRPr sz="1600" baseline="0">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -292,6 +308,37 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
       </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="80C080"/>
+            </a:gs>
+            <a:gs pos="42857">
+              <a:srgbClr val="80C080"/>
+            </a:gs>
+            <a:gs pos="42857">
+              <a:srgbClr val="FFFF80"/>
+            </a:gs>
+            <a:gs pos="57142">
+              <a:srgbClr val="FFFF80"/>
+            </a:gs>
+            <a:gs pos="57142">
+              <a:srgbClr val="FFD280"/>
+            </a:gs>
+            <a:gs pos="71428">
+              <a:srgbClr val="FFD280"/>
+            </a:gs>
+            <a:gs pos="71428">
+              <a:srgbClr val="FF8080"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="FF8080"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -313,10 +360,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -645,7 +692,7 @@
         <v>2012</v>
       </c>
       <c r="B2" s="1">
-        <v>4.581090895547403</v>
+        <v>4.562468574833796</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -653,7 +700,7 @@
         <v>2013</v>
       </c>
       <c r="B3" s="1">
-        <v>4.581103570702121</v>
+        <v>4.585883614711811</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -661,7 +708,7 @@
         <v>2014</v>
       </c>
       <c r="B4" s="1">
-        <v>4.612300651043976</v>
+        <v>4.576821415266715</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -669,7 +716,7 @@
         <v>2015</v>
       </c>
       <c r="B5" s="1">
-        <v>4.674182018146825</v>
+        <v>4.669026670332691</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -677,7 +724,7 @@
         <v>2016</v>
       </c>
       <c r="B6" s="1">
-        <v>4.672935947192092</v>
+        <v>4.660496898530534</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -685,7 +732,7 @@
         <v>2017</v>
       </c>
       <c r="B7" s="1">
-        <v>4.833134684147796</v>
+        <v>4.814628944231855</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -701,7 +748,7 @@
         <v>2019</v>
       </c>
       <c r="B9" s="1">
-        <v>5.05750889044296</v>
+        <v>5.021798324579286</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -709,7 +756,7 @@
         <v>2020</v>
       </c>
       <c r="B10" s="1">
-        <v>5.306948779540584</v>
+        <v>5.250061130848784</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -717,7 +764,7 @@
         <v>2021</v>
       </c>
       <c r="B11" s="1">
-        <v>5.728086415456785</v>
+        <v>5.71089519620262</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -725,7 +772,7 @@
         <v>2022</v>
       </c>
       <c r="B12" s="1">
-        <v>6.008419441255263</v>
+        <v>6.070443538276786</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -733,7 +780,7 @@
         <v>2023</v>
       </c>
       <c r="B13" s="1">
-        <v>6.294934746091226</v>
+        <v>6.294934746091227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>